<commit_message>
added futures to model, removed avg_price
</commit_message>
<xml_diff>
--- a/data/exog_for_pred.xlsx
+++ b/data/exog_for_pred.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nicole Dropbox\Dropbox\_GEORGETOWN Dropbox\_Hoya1\Hoya1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE19545D-DFEC-459B-BA9C-3A6501C11EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C9129C-BC02-4FD4-8467-0DAF2D91B7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{9CAE8659-7B59-AA4F-BB00-6CE9DF87B926}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="36930" windowHeight="10710" activeTab="5" xr2:uid="{9CAE8659-7B59-AA4F-BB00-6CE9DF87B926}"/>
   </bookViews>
   <sheets>
     <sheet name="OLD" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="financial_pred" sheetId="7" r:id="rId3"/>
     <sheet name="misc_pred" sheetId="8" r:id="rId4"/>
     <sheet name="financial_diffs" sheetId="9" r:id="rId5"/>
+    <sheet name="true_values" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="33">
   <si>
     <t>avg_price_all</t>
   </si>
@@ -136,6 +137,9 @@
   <si>
     <t>percentile</t>
   </si>
+  <si>
+    <t>min_temp</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +190,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -195,6 +199,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4935,7 +4940,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
@@ -5895,7 +5900,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A21"/>
+      <selection sqref="A1:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -7272,7 +7277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C389C3F-03FB-42FC-AB63-13E61D221449}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
@@ -7596,11 +7601,11 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M4:M15" si="2">M6+G7</f>
+        <f t="shared" ref="M7:M14" si="2">M6+G7</f>
         <v>74.305628520205673</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N3:N15" si="3">N6+G7</f>
+        <f t="shared" ref="N7:N15" si="3">N6+G7</f>
         <v>77.015914240205689</v>
       </c>
     </row>
@@ -8240,11 +8245,11 @@
         <v>1</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M18:M29" si="6">M20+G21</f>
+        <f t="shared" ref="M21:M29" si="6">M20+G21</f>
         <v>2899.8521387283199</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="N17:N29" si="7">N20+G21</f>
+        <f t="shared" ref="N21:N29" si="7">N20+G21</f>
         <v>2961.6801387283203</v>
       </c>
     </row>
@@ -8838,11 +8843,11 @@
         <v>2</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M32:M37" si="10">M33+G34</f>
+        <f t="shared" ref="M34:M37" si="10">M33+G34</f>
         <v>97.409308681931947</v>
       </c>
       <c r="N34">
-        <f t="shared" ref="N31:N43" si="11">N33+G34</f>
+        <f t="shared" ref="N34:N43" si="11">N33+G34</f>
         <v>98.597308681931949</v>
       </c>
     </row>
@@ -9436,11 +9441,11 @@
         <v>3</v>
       </c>
       <c r="M47">
-        <f t="shared" ref="M46:M51" si="14">M46+G47</f>
+        <f t="shared" ref="M47:M51" si="14">M46+G47</f>
         <v>26231.639154802207</v>
       </c>
       <c r="N47">
-        <f t="shared" ref="N45:N57" si="15">N46+G47</f>
+        <f t="shared" ref="N47:N57" si="15">N46+G47</f>
         <v>26764.54315480221</v>
       </c>
     </row>
@@ -10130,7 +10135,7 @@
         <v>39.712000000000003</v>
       </c>
       <c r="N62">
-        <f t="shared" ref="N59:N71" si="19">N61+G62</f>
+        <f t="shared" ref="N62:N71" si="19">N61+G62</f>
         <v>40.968000000000004</v>
       </c>
     </row>
@@ -10559,7 +10564,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -11241,4 +11246,411 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA364CF8-8416-4A1E-AF1D-13938A14748C}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="4">
+        <v>43581</v>
+      </c>
+      <c r="B2">
+        <v>1.1154999999999999</v>
+      </c>
+      <c r="C2">
+        <v>30031</v>
+      </c>
+      <c r="D2">
+        <v>99.2</v>
+      </c>
+      <c r="E2">
+        <v>10.3</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2939.88</v>
+      </c>
+      <c r="H2">
+        <v>98.01</v>
+      </c>
+      <c r="I2">
+        <v>26543.33</v>
+      </c>
+      <c r="J2">
+        <v>40.03</v>
+      </c>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="4">
+        <v>43582</v>
+      </c>
+      <c r="B3">
+        <v>1.1156999999999999</v>
+      </c>
+      <c r="C3">
+        <v>30031</v>
+      </c>
+      <c r="D3">
+        <v>99.2</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="4">
+        <v>43583</v>
+      </c>
+      <c r="B4">
+        <v>1.115</v>
+      </c>
+      <c r="C4">
+        <v>30031</v>
+      </c>
+      <c r="D4">
+        <v>99.2</v>
+      </c>
+      <c r="E4">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="4">
+        <v>43584</v>
+      </c>
+      <c r="B5">
+        <v>1.1184000000000001</v>
+      </c>
+      <c r="C5">
+        <v>30031</v>
+      </c>
+      <c r="D5">
+        <v>99.2</v>
+      </c>
+      <c r="E5">
+        <v>7.4</v>
+      </c>
+      <c r="G5">
+        <v>2943.03</v>
+      </c>
+      <c r="H5">
+        <v>97.86</v>
+      </c>
+      <c r="I5">
+        <v>26554.39</v>
+      </c>
+      <c r="J5">
+        <v>39.950000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="4">
+        <v>43585</v>
+      </c>
+      <c r="B6">
+        <v>1.1212</v>
+      </c>
+      <c r="C6">
+        <v>30031</v>
+      </c>
+      <c r="D6">
+        <v>99.2</v>
+      </c>
+      <c r="E6">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G6">
+        <v>2945.83</v>
+      </c>
+      <c r="H6">
+        <v>97.48</v>
+      </c>
+      <c r="I6">
+        <v>26592.91</v>
+      </c>
+      <c r="J6">
+        <v>39.979999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="4">
+        <v>43586</v>
+      </c>
+      <c r="B7">
+        <v>1.1203000000000001</v>
+      </c>
+      <c r="C7">
+        <v>29876</v>
+      </c>
+      <c r="D7">
+        <v>99.2</v>
+      </c>
+      <c r="E7">
+        <v>6.8</v>
+      </c>
+      <c r="G7">
+        <v>2923.73</v>
+      </c>
+      <c r="H7">
+        <v>97.69</v>
+      </c>
+      <c r="I7">
+        <v>26430.14</v>
+      </c>
+      <c r="J7">
+        <v>39.76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="4">
+        <v>43587</v>
+      </c>
+      <c r="B8">
+        <v>1.1174999999999999</v>
+      </c>
+      <c r="C8">
+        <v>29876</v>
+      </c>
+      <c r="D8">
+        <v>99.2</v>
+      </c>
+      <c r="E8">
+        <v>2.9</v>
+      </c>
+      <c r="G8">
+        <v>2917.52</v>
+      </c>
+      <c r="H8">
+        <v>97.83</v>
+      </c>
+      <c r="I8">
+        <v>26307.79</v>
+      </c>
+      <c r="J8">
+        <v>39.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="4">
+        <v>43588</v>
+      </c>
+      <c r="B9">
+        <v>1.1207</v>
+      </c>
+      <c r="C9">
+        <v>29876</v>
+      </c>
+      <c r="D9">
+        <v>99.2</v>
+      </c>
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="G9">
+        <v>2945.64</v>
+      </c>
+      <c r="H9">
+        <v>97.52</v>
+      </c>
+      <c r="I9">
+        <v>26504.95</v>
+      </c>
+      <c r="J9">
+        <v>40.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B10">
+        <v>1.1207</v>
+      </c>
+      <c r="C10">
+        <v>29876</v>
+      </c>
+      <c r="D10">
+        <v>99.2</v>
+      </c>
+      <c r="E10">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="4">
+        <v>43590</v>
+      </c>
+      <c r="B11">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C11">
+        <v>29876</v>
+      </c>
+      <c r="D11">
+        <v>99.2</v>
+      </c>
+      <c r="E11">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="4">
+        <v>43591</v>
+      </c>
+      <c r="B12">
+        <v>1.1197999999999999</v>
+      </c>
+      <c r="C12">
+        <v>29876</v>
+      </c>
+      <c r="D12">
+        <v>99.2</v>
+      </c>
+      <c r="E12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G12">
+        <v>2932.47</v>
+      </c>
+      <c r="H12">
+        <v>97.52</v>
+      </c>
+      <c r="I12">
+        <v>26438.48</v>
+      </c>
+      <c r="J12">
+        <v>39.47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="4">
+        <v>43592</v>
+      </c>
+      <c r="B13">
+        <v>1.1193</v>
+      </c>
+      <c r="C13">
+        <v>29876</v>
+      </c>
+      <c r="D13">
+        <v>99.2</v>
+      </c>
+      <c r="E13">
+        <v>1.7</v>
+      </c>
+      <c r="G13">
+        <v>2884.05</v>
+      </c>
+      <c r="H13">
+        <v>97.63</v>
+      </c>
+      <c r="I13">
+        <v>25965.09</v>
+      </c>
+      <c r="J13">
+        <v>38.729999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="4">
+        <v>43593</v>
+      </c>
+      <c r="B14">
+        <v>1.1197999999999999</v>
+      </c>
+      <c r="C14">
+        <v>29876</v>
+      </c>
+      <c r="D14">
+        <v>99.2</v>
+      </c>
+      <c r="E14">
+        <v>0.8</v>
+      </c>
+      <c r="G14">
+        <v>2879.42</v>
+      </c>
+      <c r="H14">
+        <v>97.62</v>
+      </c>
+      <c r="I14">
+        <v>25967.33</v>
+      </c>
+      <c r="J14">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="4">
+        <v>43594</v>
+      </c>
+      <c r="B15">
+        <v>1.1220000000000001</v>
+      </c>
+      <c r="C15">
+        <v>29876</v>
+      </c>
+      <c r="D15">
+        <v>99.2</v>
+      </c>
+      <c r="E15">
+        <v>2.7</v>
+      </c>
+      <c r="G15">
+        <v>2870.72</v>
+      </c>
+      <c r="H15">
+        <v>97.37</v>
+      </c>
+      <c r="I15">
+        <v>25828.36</v>
+      </c>
+      <c r="J15">
+        <v>38.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>